<commit_message>
updated BOM with assembly status, initial bluetooth audio code on PCB
</commit_message>
<xml_diff>
--- a/LPEDT_Pulse_FINAL_BOM.xlsx
+++ b/LPEDT_Pulse_FINAL_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhir\Downloads\LPEDT_Pulse_PCB_FINAL_SUBMISSION\LPEDT_Pulse_PCB_FINAL_SUBMISSION\LPEDT_Pulse_Project\BOM Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhirath_CU_Boulder_Files\Fall 2025 Sem\Low Power\ESP32-Solar-BT-Speaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27E209F8-3110-4E50-B618-B226477ABA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D16B5C-9BC0-443B-B5CB-FB32B526B7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21924" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{36E66E78-55C3-4C08-9AC0-271D19779CAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{36E66E78-55C3-4C08-9AC0-271D19779CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="LPEDT_Pulse_Project_PCB_FINAL_5" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
   <si>
     <t>Comment</t>
   </si>
@@ -422,124 +422,136 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
+    <t>Res Thick Film 0603 1K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD T/R Automotive AEC-Q200</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K00</t>
+  </si>
+  <si>
+    <t>22.1kΩ</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 22.1K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD Automotive T/R</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>RMCF0603FT22K1</t>
+  </si>
+  <si>
+    <t>47.5kΩ</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 47.5K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD T/R Automotive AEC-Q200</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>RMCF0603FT47K5</t>
+  </si>
+  <si>
+    <t>3k</t>
+  </si>
+  <si>
+    <t>3k ohm</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>RMCF0603JT3K00</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 24V</t>
+  </si>
+  <si>
+    <t>SW1, SW2, SW3</t>
+  </si>
+  <si>
+    <t>1825910-6_BUTTON</t>
+  </si>
+  <si>
+    <t>1825910-6</t>
+  </si>
+  <si>
+    <t>MAX98357A Audio Amplifier</t>
+  </si>
+  <si>
+    <t>MAX98357A Series 5.5 V 3.2 W PCM Input Class D Audio Power Amplifier - TQFN-16</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>MAX98357_QFN_T1633_4</t>
+  </si>
+  <si>
+    <t>MAX98357AETE+T</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E-N4</t>
+  </si>
+  <si>
+    <t>WLAN+BT Module 2412MHz to 2484MHz 47-Pin SMD Module</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E4</t>
+  </si>
+  <si>
+    <t>BQ25798RQMR</t>
+  </si>
+  <si>
+    <t>IÂ²C controlled, 1-4-cell, 5-A buck-boost solar battery charger with dual-input selector and MPPT</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>TPS63020DSJR</t>
+  </si>
+  <si>
+    <t>High Efficiency Single Inductor Buck-Boost Converter with 4A Switch</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>IC_TPS63020DSJR</t>
+  </si>
+  <si>
+    <t>CP2102N-A02-GQFN28R</t>
+  </si>
+  <si>
+    <t>Interface IC full speed USB to UART bridge USB 2.0 3.3V, CP2102N-A02-GQFN24R, VFQFN-24</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>IC_CP2102N-A02-GQFN28R</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>NOT DONE</t>
+  </si>
+  <si>
+    <t>NOT SURE OF ORIENTATION</t>
+  </si>
+  <si>
+    <t>PARTIAL</t>
+  </si>
+  <si>
     <t>1kΩ</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0603 1K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD T/R Automotive AEC-Q200</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>RMCF0603FT1K00</t>
-  </si>
-  <si>
-    <t>22.1kΩ</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0603 22.1K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD Automotive T/R</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>RMCF0603FT22K1</t>
-  </si>
-  <si>
-    <t>47.5kΩ</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0603 47.5K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD T/R Automotive AEC-Q200</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>RMCF0603FT47K5</t>
-  </si>
-  <si>
-    <t>3k</t>
-  </si>
-  <si>
-    <t>3k ohm</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>RMCF0603JT3K00</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 24V</t>
-  </si>
-  <si>
-    <t>SW1, SW2, SW3</t>
-  </si>
-  <si>
-    <t>1825910-6_BUTTON</t>
-  </si>
-  <si>
-    <t>1825910-6</t>
-  </si>
-  <si>
-    <t>MAX98357A Audio Amplifier</t>
-  </si>
-  <si>
-    <t>MAX98357A Series 5.5 V 3.2 W PCM Input Class D Audio Power Amplifier - TQFN-16</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>MAX98357_QFN_T1633_4</t>
-  </si>
-  <si>
-    <t>MAX98357AETE+T</t>
-  </si>
-  <si>
-    <t>ESP32-WROOM-32E-N4</t>
-  </si>
-  <si>
-    <t>WLAN+BT Module 2412MHz to 2484MHz 47-Pin SMD Module</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>ESP32-WROOM-32E4</t>
-  </si>
-  <si>
-    <t>BQ25798RQMR</t>
-  </si>
-  <si>
-    <t>IÂ²C controlled, 1-4-cell, 5-A buck-boost solar battery charger with dual-input selector and MPPT</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>TPS63020DSJR</t>
-  </si>
-  <si>
-    <t>High Efficiency Single Inductor Buck-Boost Converter with 4A Switch</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>IC_TPS63020DSJR</t>
-  </si>
-  <si>
-    <t>CP2102N-A02-GQFN28R</t>
-  </si>
-  <si>
-    <t>Interface IC full speed USB to UART bridge USB 2.0 3.3V, CP2102N-A02-GQFN24R, VFQFN-24</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>IC_CP2102N-A02-GQFN28R</t>
   </si>
 </sst>
 </file>
@@ -555,7 +567,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,8 +580,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -592,16 +616,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,16 +992,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB91E84B-7B89-41DA-B291-596651816D78}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="104" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="98.44140625" customWidth="1"/>
+    <col min="3" max="3" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="39.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -965,14 +1030,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -984,15 +1049,21 @@
       <c r="F2" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1004,15 +1075,21 @@
       <c r="F3" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1024,15 +1101,21 @@
       <c r="F4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1044,15 +1127,21 @@
       <c r="F5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1064,48 +1153,63 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="G6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1124,8 +1228,14 @@
       <c r="F9" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -1144,8 +1254,14 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1164,8 +1280,14 @@
       <c r="F11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1184,8 +1306,14 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -1204,8 +1332,14 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1224,8 +1358,17 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1244,8 +1387,14 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
@@ -1264,8 +1413,14 @@
       <c r="F16" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1284,8 +1439,14 @@
       <c r="F17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>77</v>
       </c>
@@ -1304,8 +1465,14 @@
       <c r="F18" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>82</v>
       </c>
@@ -1324,8 +1491,14 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>87</v>
       </c>
@@ -1344,8 +1517,14 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>91</v>
       </c>
@@ -1364,15 +1543,21 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1384,8 +1569,14 @@
       <c r="F22" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
@@ -1404,8 +1595,14 @@
       <c r="F23" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>103</v>
       </c>
@@ -1424,8 +1621,14 @@
       <c r="F24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>107</v>
       </c>
@@ -1444,8 +1647,14 @@
       <c r="F25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>111</v>
       </c>
@@ -1464,8 +1673,14 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>115</v>
       </c>
@@ -1484,8 +1699,14 @@
       <c r="F27" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>119</v>
       </c>
@@ -1504,15 +1725,21 @@
       <c r="F28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1524,209 +1751,275 @@
       <c r="F29" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="F34" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>